<commit_message>
close #94 - Inserimento dati costi
</commit_message>
<xml_diff>
--- a/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/graficiProcessiOrganizzativi.xlsx
+++ b/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/graficiProcessiOrganizzativi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Università\Terzo anno\SWE\Progetto\Documentazione\DocumentazioneEsterna\PianoDiQualifica\res\ResocontoAttivitaDiVerifica\res\metriche\grafici\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9390C7-C400-4E41-8FBF-E1054A2FB7CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A0B221-85BC-4E84-A720-FEA258EC3712}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{32F62035-8081-4F2C-A1C6-0EA80AA4F9D3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{32F62035-8081-4F2C-A1C6-0EA80AA4F9D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Pianificazione" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
   <si>
     <t>Accettabile</t>
   </si>
@@ -121,10 +121,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
     <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     <numFmt numFmtId="166" formatCode="&quot;€&quot;\ #,##0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -260,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -300,6 +301,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -361,8 +364,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.42440285806223998"/>
-          <c:y val="2.2650056625141562E-2"/>
+          <c:x val="0.44677305714084409"/>
+          <c:y val="2.2650197170030157E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -397,6 +400,154 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Pianificazione!$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accettabile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Pianificazione!$B$6:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PD</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Pianificazione!$D$6:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>13154</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13154</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-980B-4A83-84DA-8F4A5B1DE794}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Pianificazione!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ottimale</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Pianificazione!$B$6:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PD</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Pianificazione!$E$6:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4482</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-980B-4A83-84DA-8F4A5B1DE794}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="365907192"/>
+        <c:axId val="365909112"/>
+      </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -524,7 +675,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4280</c:v>
+                  <c:v>4417</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -533,278 +684,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-980B-4A83-84DA-8F4A5B1DE794}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Pianificazione!$D$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Accettabile</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Pianificazione!$B$6:$B$10</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>PA</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>PD</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>VC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Pianificazione!$D$6:$D$10</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13154</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-980B-4A83-84DA-8F4A5B1DE794}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Pianificazione!$E$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ottimale</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Pianificazione!$B$6:$B$10</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>PA</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>PD</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>VC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Pianificazione!$E$6:$E$10</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4482</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-980B-4A83-84DA-8F4A5B1DE794}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -931,7 +810,7 @@
         <c:axId val="365909112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="15000"/>
+          <c:max val="20000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1166,8 +1045,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.42440285806223998"/>
-          <c:y val="2.2650056625141562E-2"/>
+          <c:x val="0.39084760093003595"/>
+          <c:y val="2.2650197170030157E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1202,6 +1081,154 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Pianificazione!$D$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accettabile </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Pianificazione!$B$31:$B$34</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PD</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Pianificazione!$D$31:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4706.1000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0462-40BE-8A87-33B44F091159}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Pianificazione!$E$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ottimale</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Pianificazione!$B$31:$B$34</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PD</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Pianificazione!$E$31:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4482</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0462-40BE-8A87-33B44F091159}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="365907192"/>
+        <c:axId val="365909112"/>
+      </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1330,7 +1357,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4280</c:v>
+                  <c:v>4417</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1339,280 +1366,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0462-40BE-8A87-33B44F091159}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Pianificazione!$D$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Accettabile </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Pianificazione!$B$31:$B$34</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>PA</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>PD</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>VC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Pianificazione!$D$31:$D$34</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4706.1000000000004</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0462-40BE-8A87-33B44F091159}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Pianificazione!$E$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ottimale</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Pianificazione!$B$31:$B$34</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>PA</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>PD</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>VC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Pianificazione!$E$31:$E$34</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4482</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0462-40BE-8A87-33B44F091159}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1739,7 +1492,7 @@
         <c:axId val="365909112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="5000"/>
+          <c:max val="8000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1847,7 +1600,7 @@
         <c:crossAx val="365907192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="500"/>
+        <c:majorUnit val="1000"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1863,9 +1616,7 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent6"/>
-          </a:solidFill>
+          <a:noFill/>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -1971,8 +1722,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.42440285806223998"/>
-          <c:y val="2.2650056625141562E-2"/>
+          <c:x val="0.37742549143944198"/>
+          <c:y val="2.2650197170030157E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2048,9 +1799,80 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-4CC3-41F8-A162-36DF2CC34A3B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$61:$B$65</c:f>
+              <c:f>Pianificazione!$B$61:$B$64</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2070,15 +1892,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$C$61:$C$65</c:f>
+              <c:f>Pianificazione!$C$61:$C$64</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="0%">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0199999999999999E-2</c:v>
+                  <c:v>6.4999999999999997E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2213,6 +2035,7 @@
         <c:axId val="365909112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3.0000000000000006E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2230,61 +2053,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="it-IT"/>
-                  <a:t>Percentuale</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="it-IT"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2319,6 +2087,7 @@
         <c:crossAx val="365907192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0000000000000002E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2989,6 +2758,63 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Pianificazione!$B$104:$B$107</c:f>
@@ -3013,13 +2839,13 @@
             <c:numRef>
               <c:f>Pianificazione!$C$104:$C$107</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]">
+                <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3154,6 +2980,7 @@
         <c:axId val="365909112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="90"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3372,7 +3199,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>Metriche</a:t>
+              <a:t>Percentuale metriche</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="it-IT" baseline="0"/>
@@ -3386,8 +3213,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38008971182885742"/>
-          <c:y val="2.2650056625141562E-2"/>
+          <c:x val="0.30179401817797508"/>
+          <c:y val="2.2650197170030157E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3422,8 +3249,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -3440,29 +3268,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
               <a:solidFill>
                 <a:schemeClr val="tx2"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -3493,7 +3309,6 @@
                 <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -3556,7 +3371,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2501-4B97-B0E8-349D24C99A1B}"/>
@@ -3564,9 +3378,171 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="400"/>
+        <c:axId val="365907192"/>
+        <c:axId val="365909112"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GestioneQualità!$E$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accettabile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>GestioneQualità!$C$7:$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PD</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>GestioneQualità!$E$7:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5981-4EE5-84A6-C6AB286D5B95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GestioneQualità!$F$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ottimale</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>GestioneQualità!$C$7:$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PD</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>GestioneQualità!$F$7:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5981-4EE5-84A6-C6AB286D5B95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -3632,7 +3608,7 @@
         <c:axId val="365909112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2"/>
+          <c:max val="1.2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3693,6 +3669,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -7073,13 +7080,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>480360</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>42660</xdr:rowOff>
+      <xdr:rowOff>80760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7147,15 +7154,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1653540</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>114600</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>179820</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>175560</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>164580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7265,16 +7272,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>221280</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>65520</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>137460</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>172200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7603,8 +7610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEB098D-590A-4332-807C-B47041EA10F7}">
   <dimension ref="B4:F107"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="B118" workbookViewId="0">
+      <selection activeCell="O69" sqref="O69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7649,7 +7656,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="9">
-        <v>0</v>
+        <v>13154</v>
       </c>
       <c r="E6" s="9">
         <v>0</v>
@@ -7663,7 +7670,7 @@
         <v>24</v>
       </c>
       <c r="C7" s="9">
-        <v>4280</v>
+        <v>4417</v>
       </c>
       <c r="D7" s="9">
         <f>C13</f>
@@ -7777,7 +7784,7 @@
         <v>24</v>
       </c>
       <c r="C32" s="9">
-        <v>4280</v>
+        <v>4417</v>
       </c>
       <c r="D32" s="9">
         <f>F32+(F32*5/100)</f>
@@ -7788,6 +7795,7 @@
         <v>4482</v>
       </c>
       <c r="F32" s="32">
+        <f>F7</f>
         <v>4482</v>
       </c>
     </row>
@@ -7854,12 +7862,12 @@
       <c r="B62" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C62" s="37">
-        <v>2.0199999999999999E-2</v>
-      </c>
-      <c r="D62" s="32">
+      <c r="C62" s="40">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="D62" s="39">
         <f>(F32-C32)/100</f>
-        <v>2.02</v>
+        <v>0.65</v>
       </c>
       <c r="E62" s="17"/>
       <c r="F62" s="17"/>
@@ -8018,7 +8026,7 @@
         <v>15</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="2:5">
@@ -8039,15 +8047,17 @@
       <c r="B105" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C105" s="33">
-        <f>E105-D105</f>
-        <v>0</v>
+      <c r="C105" s="9">
+        <f>D105-E105</f>
+        <v>65</v>
       </c>
       <c r="D105" s="9">
+        <f>F7</f>
         <v>4482</v>
       </c>
       <c r="E105" s="9">
-        <v>4482</v>
+        <f>C7</f>
+        <v>4417</v>
       </c>
     </row>
     <row r="106" spans="2:5">
@@ -8075,10 +8085,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A007753-E669-4835-90BB-B57BBACA4DE7}">
-  <dimension ref="C5:G21"/>
+  <dimension ref="C5:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8087,9 +8097,11 @@
     <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.109375" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:8">
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
@@ -8098,7 +8110,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="3:7">
+    <row r="6" spans="3:8">
       <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
@@ -8106,67 +8118,92 @@
         <v>18</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="3:7">
+    <row r="7" spans="3:8">
       <c r="C7" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="19">
-        <f>E7/F7</f>
+        <f>G7/H7</f>
         <v>1</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="F7" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="G7" s="24">
         <v>3</v>
       </c>
-      <c r="F7" s="24">
+      <c r="H7" s="24">
         <v>3</v>
       </c>
-      <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="3:7">
+    <row r="8" spans="3:8">
       <c r="C8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="19">
-        <f>E8/F8</f>
+        <f>G8/H8</f>
         <v>1</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="F8" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="G8" s="24">
         <v>8</v>
       </c>
-      <c r="F8" s="24">
+      <c r="H8" s="24">
         <v>8</v>
       </c>
-      <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="3:7">
+    <row r="9" spans="3:8">
       <c r="C9" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="18"/>
+      <c r="E9" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="F9" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="3:7">
+    <row r="10" spans="3:8">
       <c r="C10" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="18"/>
+      <c r="E10" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="3:7">
+    <row r="11" spans="3:8">
       <c r="G11" s="18"/>
     </row>
-    <row r="15" spans="3:7">
+    <row r="15" spans="3:8">
       <c r="C15" s="15"/>
     </row>
     <row r="17" spans="6:6">

</xml_diff>